<commit_message>
Major refactoring of code
Changed code to separate logic from generation of output.
</commit_message>
<xml_diff>
--- a/Data_files/appointments.xlsx
+++ b/Data_files/appointments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7460" yWindow="6220" windowWidth="21680" windowHeight="10160" tabRatio="500"/>
+    <workbookView xWindow="9820" yWindow="6640" windowWidth="21680" windowHeight="10160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>